<commit_message>
add  error log to stock
</commit_message>
<xml_diff>
--- a/database/industries/methanol/shekhark/income/quarterly/rial.xlsx
+++ b/database/industries/methanol/shekhark/income/quarterly/rial.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\methanol\shekhark\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\methanol\shekhark\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78303676-E34B-4E26-8D5D-3CC5EE7FAF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="2745" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -127,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -587,12 +586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
@@ -601,7 +602,7 @@
     <col min="6" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -610,7 +611,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -621,7 +622,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -632,7 +633,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -641,7 +642,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:8" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -652,7 +653,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:8" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -663,7 +664,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -672,7 +673,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -693,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -714,7 +715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -723,7 +724,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -744,7 +745,7 @@
         <v>30259860</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
@@ -765,7 +766,7 @@
         <v>-20510752</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
@@ -786,7 +787,7 @@
         <v>9749108</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
@@ -807,7 +808,7 @@
         <v>-2683855</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
@@ -828,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>21</v>
       </c>
@@ -849,7 +850,7 @@
         <v>707235</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>22</v>
       </c>
@@ -870,7 +871,7 @@
         <v>7772488</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
@@ -891,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>24</v>
       </c>
@@ -912,7 +913,7 @@
         <v>289399</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
         <v>25</v>
       </c>
@@ -933,7 +934,7 @@
         <v>8061887</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>26</v>
       </c>
@@ -954,7 +955,7 @@
         <v>-1653672</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>27</v>
       </c>
@@ -975,7 +976,7 @@
         <v>6408215</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>28</v>
       </c>
@@ -996,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>29</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>6408215</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1056,10 +1057,10 @@
         <v>6000000</v>
       </c>
       <c r="H26" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>33</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>

</xml_diff>